<commit_message>
added upload table feature
</commit_message>
<xml_diff>
--- a/Excel_folder/TATA_2.xlsx
+++ b/Excel_folder/TATA_2.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>PARBATI HOLDINGS LTD</t>
+          <t>TATA STEEL LIMITED</t>
         </is>
       </c>
       <c r="C1" s="2" t="n"/>
@@ -534,10 +534,10 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>129006.62</v>
+        <v>1290066200000</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>129021.35</v>
+        <v>1290213500000</v>
       </c>
       <c r="D9" s="2" t="n"/>
       <c r="E9" s="2" t="n"/>
@@ -560,10 +560,10 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>3325.48</v>
+        <v>33254800000</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>1452.02</v>
+        <v>14520200000</v>
       </c>
       <c r="D11" s="2" t="n"/>
       <c r="E11" s="2" t="n"/>
@@ -575,10 +575,10 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>132332.1</v>
+        <v>1323321000000</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>130473.37</v>
+        <v>1304733700000</v>
       </c>
       <c r="D12" s="2" t="n"/>
       <c r="E12" s="2" t="n"/>
@@ -652,10 +652,10 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>243.92</v>
+        <v>2439200000</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>243.92</v>
+        <v>2439200000</v>
       </c>
       <c r="D19" s="2" t="n"/>
       <c r="E19" s="2" t="n"/>
@@ -667,10 +667,10 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>2720.71</v>
+        <v>27207100000</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>943</v>
+        <v>9430000000</v>
       </c>
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
@@ -825,10 +825,10 @@
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>3792.14</v>
+        <v>37921400000</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>2792.08</v>
+        <v>27920800000</v>
       </c>
       <c r="D34" s="2" t="n"/>
       <c r="E34" s="2" t="n"/>
@@ -1181,10 +1181,10 @@
         </is>
       </c>
       <c r="B66" s="2" t="n">
-        <v>6616.29</v>
+        <v>66162900000</v>
       </c>
       <c r="C66" s="2" t="n">
-        <v>6365.8</v>
+        <v>63658000000</v>
       </c>
       <c r="D66" s="2" t="n"/>
       <c r="E66" s="2" t="n"/>

</xml_diff>